<commit_message>
Subida versión final de la Tarea de Ordenamiento, incluidos datos, exe, ppt y arreglos visuales a los programas.
</commit_message>
<xml_diff>
--- a/Tarea Ordenamiento/Data.xlsx
+++ b/Tarea Ordenamiento/Data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/23e9cdde9cdda24e/Documentos/AED Codes/aed-repo/Tarea Ordenamiento/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diego\OneDrive\Documentos\AED Codes\aed-repo\Tarea Ordenamiento\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{360BF18F-09F0-4E90-95A3-A18C0F1CAF37}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{1DAD591B-7CCE-4660-BAB3-AFC0E495145F}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{360BF18F-09F0-4E90-95A3-A18C0F1CAF37}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{232987A1-90A3-4DDE-8FE1-878858C23752}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" xr2:uid="{6D4161C7-5084-4F9C-92CE-8B79BF32C50E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>n</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>10 000 000</t>
+  </si>
+  <si>
+    <t>para mañana tal vez</t>
   </si>
 </sst>
 </file>
@@ -138,13 +141,7 @@
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -161,6 +158,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -176,6 +179,1120 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-419"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Merge Sort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$3:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>237</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2538</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>26040</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>282528</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2819094</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-90D3-45B9-BD3A-6A7B72F7EE54}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Selection Sort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$3:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$3:$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1088</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>99036</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11363545</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1133694763</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>100000000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-90D3-45B9-BD3A-6A7B72F7EE54}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="826653552"/>
+        <c:axId val="824992336"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="826653552"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-419"/>
+                  <a:t>n</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-419"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-419"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="824992336"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="824992336"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="30000000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-419"/>
+                  <a:t>Time (microseconds)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-419"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-419"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="826653552"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-419"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-419"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -531,6 +1648,350 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>838200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1905000</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>150686</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60602A71-A158-400B-8FE5-8138C21EB32C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3324225" y="3124200"/>
+          <a:ext cx="1866900" cy="903161"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1913627</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0510E00A-9AC9-40F3-BED7-855F56EB71EA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5210175" y="3143250"/>
+          <a:ext cx="1913627" cy="838200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1885950</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>188298</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3093996-DCCE-466E-A9EA-1612E0C4E5AC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7134225" y="3143250"/>
+          <a:ext cx="1885950" cy="1302723"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>19051</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>228903</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1866900</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>581117</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{391EB3C7-207A-475D-8D48-22F99C66EDB5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9077326" y="3372153"/>
+          <a:ext cx="1847849" cy="352214"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>38591</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>523959</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{378F94C2-9EF0-4578-8160-7B0FF7011051}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10991850" y="3333750"/>
+          <a:ext cx="1953116" cy="333459"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>304800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1891490</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>647790</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6B2DCFD-9850-4AEA-BAEF-BF72B4EDA76A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12906375" y="3448050"/>
+          <a:ext cx="1891490" cy="342990"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>272142</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>92528</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>930728</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>41501</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="18" name="Chart 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6373EADD-E563-4ED9-84C9-C391C16518B4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId15"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1905000</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>61947</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>76385</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD00426C-8274-464F-9D09-32461ABA476B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14811375" y="3276600"/>
+          <a:ext cx="2005047" cy="676460"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -833,8 +2294,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CE5830E-252F-40F6-A9A9-6902D90B4165}">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -846,146 +2307,165 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="5"/>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="3"/>
+      <c r="B1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="8"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="6"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="9"/>
+      <c r="D2" s="7"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
+      <c r="A3" s="4">
         <v>1</v>
       </c>
       <c r="B3" s="1">
         <v>0</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="9"/>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="7"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
+      <c r="A4" s="4">
         <v>10</v>
       </c>
       <c r="B4" s="1">
         <v>5</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="9"/>
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
+      <c r="D4" s="7"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
+      <c r="A5" s="4">
         <v>100</v>
       </c>
       <c r="B5" s="1">
         <v>27</v>
       </c>
-      <c r="C5" s="1"/>
+      <c r="C5" s="1">
+        <v>14</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
+      <c r="A6" s="4">
         <v>1000</v>
       </c>
       <c r="B6" s="1">
         <v>237</v>
       </c>
-      <c r="C6" s="1"/>
+      <c r="C6" s="1">
+        <v>1088</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
+      <c r="A7" s="4">
         <v>10000</v>
       </c>
       <c r="B7" s="1">
         <v>2538</v>
       </c>
-      <c r="C7" s="1"/>
+      <c r="C7" s="1">
+        <v>99036</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
+      <c r="A8" s="4">
         <v>100000</v>
       </c>
       <c r="B8" s="1">
         <v>26040</v>
       </c>
-      <c r="C8" s="1"/>
+      <c r="C8" s="1">
+        <v>11363545</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
+      <c r="A9" s="4">
         <v>1000000</v>
       </c>
       <c r="B9" s="1">
         <v>282528</v>
       </c>
-      <c r="C9" s="1"/>
+      <c r="C9" s="1">
+        <v>1133694763</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
+      <c r="A10" s="4">
         <v>10000000</v>
       </c>
       <c r="B10" s="1">
         <v>2819094</v>
       </c>
-      <c r="C10" s="1"/>
+      <c r="C10" s="1">
+        <v>100000000000</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E12" s="3">
+      <c r="E12" s="2">
         <v>1</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="2">
         <v>10</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12" s="2">
         <v>100</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="H12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I12" s="3" t="s">
+      <c r="I12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J12" s="3" t="s">
+      <c r="J12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K12" s="3" t="s">
+      <c r="K12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="L12" s="3" t="s">
+      <c r="L12" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="L13" s="10"/>
+      <c r="L13" s="8"/>
     </row>
     <row r="14" spans="1:12" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="2" t="s">
         <v>2</v>
+      </c>
+      <c r="L14" s="8" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -994,6 +2474,7 @@
     <mergeCell ref="E11:L11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>